<commit_message>
Mistake in manual gating (Freq of parent instead of count)
</commit_message>
<xml_diff>
--- a/Data/flow/BCG_Survival_Myeloid/Manual_gating.xlsx
+++ b/Data/flow/BCG_Survival_Myeloid/Manual_gating.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/_henaolab/Documents/R/Data/Methods/Data/flow/BCG_Survival_Myeloid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA71349-4831-1B40-A737-D58813346B9F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B35E77-B555-2649-BA2A-F0D6D54BBD14}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18500" yWindow="4140" windowWidth="28040" windowHeight="17440" xr2:uid="{9EE134AF-5D12-AA42-B3F8-624C15E42FB0}"/>
+    <workbookView xWindow="2780" yWindow="2440" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{9EE134AF-5D12-AA42-B3F8-624C15E42FB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>Sample:</t>
   </si>
@@ -471,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C28956A-3ED8-BD4C-8CFD-8EBC92AE7F99}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:W39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1187,4 +1188,723 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2608D41D-76E6-3241-A778-97F8E212ABB7}">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>573</v>
+      </c>
+      <c r="E2">
+        <v>219</v>
+      </c>
+      <c r="F2">
+        <v>99</v>
+      </c>
+      <c r="G2">
+        <v>340</v>
+      </c>
+      <c r="H2">
+        <v>161</v>
+      </c>
+      <c r="I2">
+        <v>1610</v>
+      </c>
+      <c r="J2">
+        <v>428</v>
+      </c>
+      <c r="K2">
+        <v>4829</v>
+      </c>
+      <c r="L2">
+        <v>268</v>
+      </c>
+      <c r="M2">
+        <v>4720</v>
+      </c>
+      <c r="N2">
+        <v>56556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>66</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>128</v>
+      </c>
+      <c r="E3">
+        <v>502</v>
+      </c>
+      <c r="F3">
+        <v>111</v>
+      </c>
+      <c r="G3">
+        <v>229</v>
+      </c>
+      <c r="H3">
+        <v>34</v>
+      </c>
+      <c r="I3">
+        <v>1316</v>
+      </c>
+      <c r="J3">
+        <v>77</v>
+      </c>
+      <c r="K3">
+        <v>3965</v>
+      </c>
+      <c r="L3">
+        <v>71</v>
+      </c>
+      <c r="M3">
+        <v>1252</v>
+      </c>
+      <c r="N3">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>152</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>184</v>
+      </c>
+      <c r="E4">
+        <v>295</v>
+      </c>
+      <c r="F4">
+        <v>111</v>
+      </c>
+      <c r="G4">
+        <v>132</v>
+      </c>
+      <c r="H4">
+        <v>44</v>
+      </c>
+      <c r="I4">
+        <v>1626</v>
+      </c>
+      <c r="J4">
+        <v>142</v>
+      </c>
+      <c r="K4">
+        <v>5453</v>
+      </c>
+      <c r="L4">
+        <v>264</v>
+      </c>
+      <c r="M4">
+        <v>3788</v>
+      </c>
+      <c r="N4">
+        <v>52815</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>570</v>
+      </c>
+      <c r="E5">
+        <v>320</v>
+      </c>
+      <c r="F5">
+        <v>113</v>
+      </c>
+      <c r="G5">
+        <v>505</v>
+      </c>
+      <c r="H5">
+        <v>227</v>
+      </c>
+      <c r="I5">
+        <v>1393</v>
+      </c>
+      <c r="J5">
+        <v>625</v>
+      </c>
+      <c r="K5">
+        <v>5259</v>
+      </c>
+      <c r="L5">
+        <v>423</v>
+      </c>
+      <c r="M5">
+        <v>5611</v>
+      </c>
+      <c r="N5">
+        <v>59917</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>54</v>
+      </c>
+      <c r="D6">
+        <v>390</v>
+      </c>
+      <c r="E6">
+        <v>334</v>
+      </c>
+      <c r="F6">
+        <v>128</v>
+      </c>
+      <c r="G6">
+        <v>274</v>
+      </c>
+      <c r="H6">
+        <v>37</v>
+      </c>
+      <c r="I6">
+        <v>1626</v>
+      </c>
+      <c r="J6">
+        <v>216</v>
+      </c>
+      <c r="K6">
+        <v>6001</v>
+      </c>
+      <c r="L6">
+        <v>324</v>
+      </c>
+      <c r="M6">
+        <v>3952</v>
+      </c>
+      <c r="N6">
+        <v>60633</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>416</v>
+      </c>
+      <c r="E7">
+        <v>315</v>
+      </c>
+      <c r="F7">
+        <v>66</v>
+      </c>
+      <c r="G7">
+        <v>746</v>
+      </c>
+      <c r="H7">
+        <v>162</v>
+      </c>
+      <c r="I7">
+        <v>1145</v>
+      </c>
+      <c r="J7">
+        <v>430</v>
+      </c>
+      <c r="K7">
+        <v>5350</v>
+      </c>
+      <c r="L7">
+        <v>198</v>
+      </c>
+      <c r="M7">
+        <v>3582</v>
+      </c>
+      <c r="N7">
+        <v>57303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>52</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>556</v>
+      </c>
+      <c r="E8">
+        <v>275</v>
+      </c>
+      <c r="F8">
+        <v>131</v>
+      </c>
+      <c r="G8">
+        <v>160</v>
+      </c>
+      <c r="H8">
+        <v>62</v>
+      </c>
+      <c r="I8">
+        <v>1144</v>
+      </c>
+      <c r="J8">
+        <v>607</v>
+      </c>
+      <c r="K8">
+        <v>3307</v>
+      </c>
+      <c r="L8">
+        <v>224</v>
+      </c>
+      <c r="M8">
+        <v>3548</v>
+      </c>
+      <c r="N8">
+        <v>53526</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>554</v>
+      </c>
+      <c r="E9">
+        <v>190</v>
+      </c>
+      <c r="F9">
+        <v>92</v>
+      </c>
+      <c r="G9">
+        <v>172</v>
+      </c>
+      <c r="H9">
+        <v>67</v>
+      </c>
+      <c r="I9">
+        <v>824</v>
+      </c>
+      <c r="J9">
+        <v>906</v>
+      </c>
+      <c r="K9">
+        <v>3268</v>
+      </c>
+      <c r="L9">
+        <v>492</v>
+      </c>
+      <c r="M9">
+        <v>4147</v>
+      </c>
+      <c r="N9">
+        <v>55164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>290</v>
+      </c>
+      <c r="E10">
+        <v>262</v>
+      </c>
+      <c r="F10">
+        <v>228</v>
+      </c>
+      <c r="G10">
+        <v>19</v>
+      </c>
+      <c r="H10">
+        <v>52</v>
+      </c>
+      <c r="I10">
+        <v>192</v>
+      </c>
+      <c r="J10">
+        <v>22</v>
+      </c>
+      <c r="K10">
+        <v>2720</v>
+      </c>
+      <c r="L10">
+        <v>312</v>
+      </c>
+      <c r="M10">
+        <v>1882</v>
+      </c>
+      <c r="N10">
+        <v>53256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>625</v>
+      </c>
+      <c r="E11">
+        <v>334</v>
+      </c>
+      <c r="F11">
+        <v>173</v>
+      </c>
+      <c r="G11">
+        <v>103</v>
+      </c>
+      <c r="H11">
+        <v>53</v>
+      </c>
+      <c r="I11">
+        <v>303</v>
+      </c>
+      <c r="J11">
+        <v>28</v>
+      </c>
+      <c r="K11">
+        <v>3338</v>
+      </c>
+      <c r="L11">
+        <v>190</v>
+      </c>
+      <c r="M11">
+        <v>1508</v>
+      </c>
+      <c r="N11">
+        <v>49643</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>51</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>488</v>
+      </c>
+      <c r="E12">
+        <v>324</v>
+      </c>
+      <c r="F12">
+        <v>137</v>
+      </c>
+      <c r="G12">
+        <v>170</v>
+      </c>
+      <c r="H12">
+        <v>50</v>
+      </c>
+      <c r="I12">
+        <v>268</v>
+      </c>
+      <c r="J12">
+        <v>37</v>
+      </c>
+      <c r="K12">
+        <v>2829</v>
+      </c>
+      <c r="L12">
+        <v>143</v>
+      </c>
+      <c r="M12">
+        <v>1543</v>
+      </c>
+      <c r="N12">
+        <v>52950</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>31</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>259</v>
+      </c>
+      <c r="E13">
+        <v>337</v>
+      </c>
+      <c r="F13">
+        <v>169</v>
+      </c>
+      <c r="G13">
+        <v>142</v>
+      </c>
+      <c r="H13">
+        <v>79</v>
+      </c>
+      <c r="I13">
+        <v>288</v>
+      </c>
+      <c r="J13">
+        <v>28</v>
+      </c>
+      <c r="K13">
+        <v>4137</v>
+      </c>
+      <c r="L13">
+        <v>113</v>
+      </c>
+      <c r="M13">
+        <v>1447</v>
+      </c>
+      <c r="N13">
+        <v>47844</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>36</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>905</v>
+      </c>
+      <c r="E14">
+        <v>231</v>
+      </c>
+      <c r="F14">
+        <v>129</v>
+      </c>
+      <c r="G14">
+        <v>183</v>
+      </c>
+      <c r="H14">
+        <v>85</v>
+      </c>
+      <c r="I14">
+        <v>775</v>
+      </c>
+      <c r="J14">
+        <v>730</v>
+      </c>
+      <c r="K14">
+        <v>3275</v>
+      </c>
+      <c r="L14">
+        <v>325</v>
+      </c>
+      <c r="M14">
+        <v>4969</v>
+      </c>
+      <c r="N14">
+        <v>60669</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>64</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>425</v>
+      </c>
+      <c r="E15">
+        <v>238</v>
+      </c>
+      <c r="F15">
+        <v>96</v>
+      </c>
+      <c r="G15">
+        <v>441</v>
+      </c>
+      <c r="H15">
+        <v>210</v>
+      </c>
+      <c r="I15">
+        <v>496</v>
+      </c>
+      <c r="J15">
+        <v>349</v>
+      </c>
+      <c r="K15">
+        <v>3957</v>
+      </c>
+      <c r="L15">
+        <v>326</v>
+      </c>
+      <c r="M15">
+        <v>4796</v>
+      </c>
+      <c r="N15">
+        <v>51203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>789</v>
+      </c>
+      <c r="E16">
+        <v>106</v>
+      </c>
+      <c r="F16">
+        <v>66</v>
+      </c>
+      <c r="G16">
+        <v>117</v>
+      </c>
+      <c r="H16">
+        <v>102</v>
+      </c>
+      <c r="I16">
+        <v>432</v>
+      </c>
+      <c r="J16">
+        <v>797</v>
+      </c>
+      <c r="K16">
+        <v>2592</v>
+      </c>
+      <c r="L16">
+        <v>720</v>
+      </c>
+      <c r="M16">
+        <v>6419</v>
+      </c>
+      <c r="N16">
+        <v>62819</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>